<commit_message>
Automatic Abs/Pres Students // UI improved
</commit_message>
<xml_diff>
--- a/src/Presentation/Virgol.School/ClientApp/public/samples/SchoolTemplate.xlsx
+++ b/src/Presentation/Virgol.School/ClientApp/public/samples/SchoolTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\VSCode\LMS Moodle\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B606D631-F86B-442B-9585-74CEB0215697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC673BA6-5343-495C-BC31-EE380F42B176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>نام مدرسه</t>
   </si>
@@ -45,7 +45,10 @@
     <t>کد پرسنلی مدیر</t>
   </si>
   <si>
-    <t>شماره تلفن مدیر</t>
+    <t>شماره تماس مدیر</t>
+  </si>
+  <si>
+    <t>جنسیت (دخترانه/پسرانه)</t>
   </si>
 </sst>
 </file>
@@ -363,23 +366,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,18 +391,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Student Mother Name Added
</commit_message>
<xml_diff>
--- a/src/Presentation/Virgol.School/ClientApp/public/samples/SchoolTemplate.xlsx
+++ b/src/Presentation/Virgol.School/ClientApp/public/samples/SchoolTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\VSCode\LMS Moodle\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\VSCode\LMS Moodle\lms-with-moodle\src\Presentation\Virgol.School\ClientApp\public\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC673BA6-5343-495C-BC31-EE380F42B176}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99EA1CA-02A7-47CE-83DA-4C0BDF411B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>

</xml_diff>